<commit_message>
Small edits to supp tables
</commit_message>
<xml_diff>
--- a/table_s1_simulated_read_results.xlsx
+++ b/table_s1_simulated_read_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/Paper_GitHub_repo/1_simulated_read_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/PAPER/GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8265CBF-9718-674E-98F7-6B3591CF5A89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586EAF7-747C-D04C-84A0-E43F71A34A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8520" yWindow="-28180" windowWidth="31620" windowHeight="16440" activeTab="3" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
+    <workbookView xWindow="-8520" yWindow="-28180" windowWidth="31620" windowHeight="16440" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="5" r:id="rId1"/>
@@ -4397,24 +4397,66 @@
     <xf numFmtId="166" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4430,12 +4472,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4543,42 +4579,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4957,9 +4957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1594AA0-EE0D-E449-A849-C4CB9380F2B1}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5020,7 +5018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8755,10 +8753,10 @@
       <c r="B1" s="203"/>
       <c r="C1" s="204"/>
       <c r="D1" s="215"/>
-      <c r="E1" s="327" t="s">
+      <c r="E1" s="339" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="327"/>
+      <c r="F1" s="339"/>
     </row>
     <row r="2" spans="1:6" ht="99" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="205" t="s">
@@ -8993,9 +8991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628223D7-2890-1641-B536-A3A951EFE8FE}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9017,24 +9013,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
-      <c r="B1" s="338" t="s">
+      <c r="B1" s="340" t="s">
         <v>918</v>
       </c>
-      <c r="C1" s="339"/>
-      <c r="D1" s="339"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="339"/>
-      <c r="G1" s="339"/>
-      <c r="H1" s="339"/>
-      <c r="I1" s="339"/>
-      <c r="J1" s="339"/>
-      <c r="K1" s="330" t="s">
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="341"/>
+      <c r="I1" s="341"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="342" t="s">
         <v>919</v>
       </c>
-      <c r="L1" s="331"/>
-      <c r="M1" s="331"/>
-      <c r="N1" s="331"/>
-      <c r="O1" s="332"/>
+      <c r="L1" s="343"/>
+      <c r="M1" s="343"/>
+      <c r="N1" s="343"/>
+      <c r="O1" s="344"/>
     </row>
     <row r="2" spans="1:15" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -9087,46 +9083,46 @@
       <c r="A3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="376" t="s">
+      <c r="B3" s="327" t="s">
         <v>940</v>
       </c>
-      <c r="C3" s="385" t="s">
+      <c r="C3" s="336" t="s">
         <v>970</v>
       </c>
-      <c r="D3" s="385" t="s">
+      <c r="D3" s="336" t="s">
         <v>941</v>
       </c>
-      <c r="E3" s="377">
+      <c r="E3" s="328">
         <v>26</v>
       </c>
-      <c r="F3" s="377">
+      <c r="F3" s="328">
         <v>15</v>
       </c>
-      <c r="G3" s="377">
+      <c r="G3" s="328">
         <v>0</v>
       </c>
-      <c r="H3" s="377">
+      <c r="H3" s="328">
         <v>0</v>
       </c>
-      <c r="I3" s="377">
+      <c r="I3" s="328">
         <v>1.2</v>
       </c>
-      <c r="J3" s="377" t="s">
+      <c r="J3" s="328" t="s">
         <v>942</v>
       </c>
-      <c r="K3" s="376" t="s">
+      <c r="K3" s="327" t="s">
         <v>925</v>
       </c>
-      <c r="L3" s="377">
+      <c r="L3" s="328">
         <v>250</v>
       </c>
-      <c r="M3" s="377">
+      <c r="M3" s="328">
         <v>90</v>
       </c>
-      <c r="N3" s="377">
+      <c r="N3" s="328">
         <v>340</v>
       </c>
-      <c r="O3" s="378">
+      <c r="O3" s="329">
         <v>53</v>
       </c>
     </row>
@@ -9134,46 +9130,46 @@
       <c r="A4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="379" t="s">
+      <c r="B4" s="330" t="s">
         <v>943</v>
       </c>
-      <c r="C4" s="386" t="s">
+      <c r="C4" s="337" t="s">
         <v>971</v>
       </c>
-      <c r="D4" s="386" t="s">
+      <c r="D4" s="337" t="s">
         <v>944</v>
       </c>
-      <c r="E4" s="380">
+      <c r="E4" s="331">
         <v>2</v>
       </c>
-      <c r="F4" s="380">
+      <c r="F4" s="331">
         <v>40</v>
       </c>
-      <c r="G4" s="380">
+      <c r="G4" s="331">
         <v>0</v>
       </c>
-      <c r="H4" s="380">
+      <c r="H4" s="331">
         <v>0</v>
       </c>
-      <c r="I4" s="380">
+      <c r="I4" s="331">
         <v>1.2</v>
       </c>
-      <c r="J4" s="380" t="s">
+      <c r="J4" s="331" t="s">
         <v>945</v>
       </c>
-      <c r="K4" s="379" t="s">
+      <c r="K4" s="330" t="s">
         <v>926</v>
       </c>
-      <c r="L4" s="380">
+      <c r="L4" s="331">
         <v>150</v>
       </c>
-      <c r="M4" s="380">
+      <c r="M4" s="331">
         <v>110</v>
       </c>
-      <c r="N4" s="380">
+      <c r="N4" s="331">
         <v>420</v>
       </c>
-      <c r="O4" s="381">
+      <c r="O4" s="332">
         <v>21</v>
       </c>
     </row>
@@ -9181,46 +9177,46 @@
       <c r="A5" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="379" t="s">
+      <c r="B5" s="330" t="s">
         <v>946</v>
       </c>
-      <c r="C5" s="386" t="s">
+      <c r="C5" s="337" t="s">
         <v>972</v>
       </c>
-      <c r="D5" s="386" t="s">
+      <c r="D5" s="337" t="s">
         <v>947</v>
       </c>
-      <c r="E5" s="380">
+      <c r="E5" s="331">
         <v>2</v>
       </c>
-      <c r="F5" s="380">
+      <c r="F5" s="331">
         <v>44</v>
       </c>
-      <c r="G5" s="380">
+      <c r="G5" s="331">
         <v>0</v>
       </c>
-      <c r="H5" s="380">
+      <c r="H5" s="331">
         <v>0</v>
       </c>
-      <c r="I5" s="380">
+      <c r="I5" s="331">
         <v>2.1</v>
       </c>
-      <c r="J5" s="380" t="s">
+      <c r="J5" s="331" t="s">
         <v>948</v>
       </c>
-      <c r="K5" s="379" t="s">
+      <c r="K5" s="330" t="s">
         <v>927</v>
       </c>
-      <c r="L5" s="380">
+      <c r="L5" s="331">
         <v>150</v>
       </c>
-      <c r="M5" s="380">
+      <c r="M5" s="331">
         <v>40</v>
       </c>
-      <c r="N5" s="380">
+      <c r="N5" s="331">
         <v>500</v>
       </c>
-      <c r="O5" s="381">
+      <c r="O5" s="332">
         <v>122</v>
       </c>
     </row>
@@ -9228,46 +9224,46 @@
       <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="379" t="s">
+      <c r="B6" s="330" t="s">
         <v>949</v>
       </c>
-      <c r="C6" s="386" t="s">
+      <c r="C6" s="337" t="s">
         <v>973</v>
       </c>
-      <c r="D6" s="386" t="s">
+      <c r="D6" s="337" t="s">
         <v>950</v>
       </c>
-      <c r="E6" s="380">
+      <c r="E6" s="331">
         <v>9</v>
       </c>
-      <c r="F6" s="380">
+      <c r="F6" s="331">
         <v>16</v>
       </c>
-      <c r="G6" s="380">
+      <c r="G6" s="331">
         <v>0</v>
       </c>
-      <c r="H6" s="380">
+      <c r="H6" s="331">
         <v>0</v>
       </c>
-      <c r="I6" s="380">
+      <c r="I6" s="331">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J6" s="380" t="s">
+      <c r="J6" s="331" t="s">
         <v>951</v>
       </c>
-      <c r="K6" s="379" t="s">
+      <c r="K6" s="330" t="s">
         <v>928</v>
       </c>
-      <c r="L6" s="380">
+      <c r="L6" s="331">
         <v>250</v>
       </c>
-      <c r="M6" s="380">
+      <c r="M6" s="331">
         <v>130</v>
       </c>
-      <c r="N6" s="380">
+      <c r="N6" s="331">
         <v>300</v>
       </c>
-      <c r="O6" s="381">
+      <c r="O6" s="332">
         <v>30</v>
       </c>
     </row>
@@ -9275,46 +9271,46 @@
       <c r="A7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="379" t="s">
+      <c r="B7" s="330" t="s">
         <v>952</v>
       </c>
-      <c r="C7" s="386" t="s">
+      <c r="C7" s="337" t="s">
         <v>974</v>
       </c>
-      <c r="D7" s="386" t="s">
+      <c r="D7" s="337" t="s">
         <v>953</v>
       </c>
-      <c r="E7" s="380">
+      <c r="E7" s="331">
         <v>2</v>
       </c>
-      <c r="F7" s="380">
+      <c r="F7" s="331">
         <v>19</v>
       </c>
-      <c r="G7" s="380">
+      <c r="G7" s="331">
         <v>0</v>
       </c>
-      <c r="H7" s="380">
+      <c r="H7" s="331">
         <v>0</v>
       </c>
-      <c r="I7" s="380">
+      <c r="I7" s="331">
         <v>2.5</v>
       </c>
-      <c r="J7" s="380" t="s">
+      <c r="J7" s="331" t="s">
         <v>954</v>
       </c>
-      <c r="K7" s="379" t="s">
+      <c r="K7" s="330" t="s">
         <v>926</v>
       </c>
-      <c r="L7" s="380">
+      <c r="L7" s="331">
         <v>125</v>
       </c>
-      <c r="M7" s="380">
+      <c r="M7" s="331">
         <v>70</v>
       </c>
-      <c r="N7" s="380">
+      <c r="N7" s="331">
         <v>460</v>
       </c>
-      <c r="O7" s="381">
+      <c r="O7" s="332">
         <v>31</v>
       </c>
     </row>
@@ -9322,46 +9318,46 @@
       <c r="A8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="379" t="s">
+      <c r="B8" s="330" t="s">
         <v>955</v>
       </c>
-      <c r="C8" s="386" t="s">
+      <c r="C8" s="337" t="s">
         <v>975</v>
       </c>
-      <c r="D8" s="386" t="s">
+      <c r="D8" s="337" t="s">
         <v>956</v>
       </c>
-      <c r="E8" s="380">
+      <c r="E8" s="331">
         <v>27</v>
       </c>
-      <c r="F8" s="380">
+      <c r="F8" s="331">
         <v>14</v>
       </c>
-      <c r="G8" s="380">
+      <c r="G8" s="331">
         <v>0</v>
       </c>
-      <c r="H8" s="380">
+      <c r="H8" s="331">
         <v>0</v>
       </c>
-      <c r="I8" s="380">
+      <c r="I8" s="331">
         <v>0.6</v>
       </c>
-      <c r="J8" s="380" t="s">
+      <c r="J8" s="331" t="s">
         <v>957</v>
       </c>
-      <c r="K8" s="379" t="s">
+      <c r="K8" s="330" t="s">
         <v>929</v>
       </c>
-      <c r="L8" s="380">
+      <c r="L8" s="331">
         <v>100</v>
       </c>
-      <c r="M8" s="380">
+      <c r="M8" s="331">
         <v>120</v>
       </c>
-      <c r="N8" s="380">
+      <c r="N8" s="331">
         <v>540</v>
       </c>
-      <c r="O8" s="381">
+      <c r="O8" s="332">
         <v>45</v>
       </c>
     </row>
@@ -9369,46 +9365,46 @@
       <c r="A9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="379" t="s">
+      <c r="B9" s="330" t="s">
         <v>958</v>
       </c>
-      <c r="C9" s="386" t="s">
+      <c r="C9" s="337" t="s">
         <v>976</v>
       </c>
-      <c r="D9" s="386" t="s">
+      <c r="D9" s="337" t="s">
         <v>959</v>
       </c>
-      <c r="E9" s="380">
+      <c r="E9" s="331">
         <v>21</v>
       </c>
-      <c r="F9" s="380">
+      <c r="F9" s="331">
         <v>2</v>
       </c>
-      <c r="G9" s="380">
+      <c r="G9" s="331">
         <v>0</v>
       </c>
-      <c r="H9" s="380">
+      <c r="H9" s="331">
         <v>0</v>
       </c>
-      <c r="I9" s="380">
+      <c r="I9" s="331">
         <v>1.9</v>
       </c>
-      <c r="J9" s="380" t="s">
+      <c r="J9" s="331" t="s">
         <v>960</v>
       </c>
-      <c r="K9" s="379" t="s">
+      <c r="K9" s="330" t="s">
         <v>926</v>
       </c>
-      <c r="L9" s="380">
+      <c r="L9" s="331">
         <v>125</v>
       </c>
-      <c r="M9" s="380">
+      <c r="M9" s="331">
         <v>80</v>
       </c>
-      <c r="N9" s="380">
+      <c r="N9" s="331">
         <v>660</v>
       </c>
-      <c r="O9" s="381">
+      <c r="O9" s="332">
         <v>51</v>
       </c>
     </row>
@@ -9416,46 +9412,46 @@
       <c r="A10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="379" t="s">
+      <c r="B10" s="330" t="s">
         <v>961</v>
       </c>
-      <c r="C10" s="386" t="s">
+      <c r="C10" s="337" t="s">
         <v>977</v>
       </c>
-      <c r="D10" s="386" t="s">
+      <c r="D10" s="337" t="s">
         <v>962</v>
       </c>
-      <c r="E10" s="380">
+      <c r="E10" s="331">
         <v>43</v>
       </c>
-      <c r="F10" s="380">
+      <c r="F10" s="331">
         <v>12</v>
       </c>
-      <c r="G10" s="380">
+      <c r="G10" s="331">
         <v>0</v>
       </c>
-      <c r="H10" s="380">
+      <c r="H10" s="331">
         <v>0</v>
       </c>
-      <c r="I10" s="380">
+      <c r="I10" s="331">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J10" s="380" t="s">
+      <c r="J10" s="331" t="s">
         <v>963</v>
       </c>
-      <c r="K10" s="379" t="s">
+      <c r="K10" s="330" t="s">
         <v>929</v>
       </c>
-      <c r="L10" s="380">
+      <c r="L10" s="331">
         <v>100</v>
       </c>
-      <c r="M10" s="380">
+      <c r="M10" s="331">
         <v>50</v>
       </c>
-      <c r="N10" s="380">
+      <c r="N10" s="331">
         <v>580</v>
       </c>
-      <c r="O10" s="381">
+      <c r="O10" s="332">
         <v>61</v>
       </c>
     </row>
@@ -9463,46 +9459,46 @@
       <c r="A11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="379" t="s">
+      <c r="B11" s="330" t="s">
         <v>964</v>
       </c>
-      <c r="C11" s="386" t="s">
+      <c r="C11" s="337" t="s">
         <v>978</v>
       </c>
-      <c r="D11" s="386" t="s">
+      <c r="D11" s="337" t="s">
         <v>965</v>
       </c>
-      <c r="E11" s="380">
+      <c r="E11" s="331">
         <v>23</v>
       </c>
-      <c r="F11" s="380">
+      <c r="F11" s="331">
         <v>14</v>
       </c>
-      <c r="G11" s="380">
+      <c r="G11" s="331">
         <v>0</v>
       </c>
-      <c r="H11" s="380">
+      <c r="H11" s="331">
         <v>0</v>
       </c>
-      <c r="I11" s="380">
+      <c r="I11" s="331">
         <v>0.4</v>
       </c>
-      <c r="J11" s="380" t="s">
+      <c r="J11" s="331" t="s">
         <v>966</v>
       </c>
-      <c r="K11" s="379" t="s">
+      <c r="K11" s="330" t="s">
         <v>926</v>
       </c>
-      <c r="L11" s="380">
+      <c r="L11" s="331">
         <v>150</v>
       </c>
-      <c r="M11" s="380">
+      <c r="M11" s="331">
         <v>60</v>
       </c>
-      <c r="N11" s="380">
+      <c r="N11" s="331">
         <v>380</v>
       </c>
-      <c r="O11" s="381">
+      <c r="O11" s="332">
         <v>81</v>
       </c>
     </row>
@@ -9510,46 +9506,46 @@
       <c r="A12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="382" t="s">
+      <c r="B12" s="333" t="s">
         <v>967</v>
       </c>
-      <c r="C12" s="387" t="s">
+      <c r="C12" s="338" t="s">
         <v>979</v>
       </c>
-      <c r="D12" s="387" t="s">
+      <c r="D12" s="338" t="s">
         <v>968</v>
       </c>
-      <c r="E12" s="383">
+      <c r="E12" s="334">
         <v>43</v>
       </c>
-      <c r="F12" s="383">
+      <c r="F12" s="334">
         <v>2</v>
       </c>
-      <c r="G12" s="383">
+      <c r="G12" s="334">
         <v>0</v>
       </c>
-      <c r="H12" s="383">
+      <c r="H12" s="334">
         <v>0</v>
       </c>
-      <c r="I12" s="383">
+      <c r="I12" s="334">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J12" s="383" t="s">
+      <c r="J12" s="334" t="s">
         <v>969</v>
       </c>
-      <c r="K12" s="382" t="s">
+      <c r="K12" s="333" t="s">
         <v>930</v>
       </c>
-      <c r="L12" s="383">
+      <c r="L12" s="334">
         <v>150</v>
       </c>
-      <c r="M12" s="383">
+      <c r="M12" s="334">
         <v>100</v>
       </c>
-      <c r="N12" s="383">
+      <c r="N12" s="334">
         <v>620</v>
       </c>
-      <c r="O12" s="384">
+      <c r="O12" s="335">
         <v>117</v>
       </c>
     </row>
@@ -9570,7 +9566,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:M13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9588,46 +9584,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="72" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="338" t="s">
+      <c r="B1" s="340" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="339"/>
-      <c r="D1" s="339"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="339"/>
-      <c r="G1" s="339"/>
-      <c r="H1" s="330" t="s">
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
+      <c r="G1" s="341"/>
+      <c r="H1" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="331"/>
-      <c r="J1" s="331"/>
-      <c r="K1" s="331"/>
-      <c r="L1" s="331"/>
-      <c r="M1" s="332"/>
+      <c r="I1" s="343"/>
+      <c r="J1" s="343"/>
+      <c r="K1" s="343"/>
+      <c r="L1" s="343"/>
+      <c r="M1" s="344"/>
     </row>
     <row r="2" spans="1:13" s="72" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="336" t="s">
+      <c r="B2" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="337"/>
-      <c r="D2" s="337"/>
-      <c r="E2" s="328" t="s">
+      <c r="C2" s="351"/>
+      <c r="D2" s="351"/>
+      <c r="E2" s="345" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="337"/>
-      <c r="G2" s="329"/>
-      <c r="H2" s="333" t="s">
+      <c r="F2" s="351"/>
+      <c r="G2" s="346"/>
+      <c r="H2" s="347" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="334"/>
-      <c r="J2" s="335" t="s">
+      <c r="I2" s="348"/>
+      <c r="J2" s="349" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="334"/>
-      <c r="L2" s="328" t="s">
+      <c r="K2" s="348"/>
+      <c r="L2" s="345" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="329"/>
+      <c r="M2" s="346"/>
     </row>
     <row r="3" spans="1:13" s="80" customFormat="1" ht="36" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -10143,41 +10139,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="124" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="345" t="s">
+      <c r="B1" s="357" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="346"/>
-      <c r="D1" s="346"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="346"/>
-      <c r="G1" s="349" t="s">
+      <c r="C1" s="358"/>
+      <c r="D1" s="358"/>
+      <c r="E1" s="358"/>
+      <c r="F1" s="358"/>
+      <c r="G1" s="361" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="350"/>
-      <c r="I1" s="350"/>
-      <c r="J1" s="350"/>
-      <c r="K1" s="350"/>
-      <c r="L1" s="347" t="s">
+      <c r="H1" s="362"/>
+      <c r="I1" s="362"/>
+      <c r="J1" s="362"/>
+      <c r="K1" s="362"/>
+      <c r="L1" s="359" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="348"/>
-      <c r="N1" s="348"/>
-      <c r="O1" s="348"/>
-      <c r="P1" s="348"/>
-      <c r="Q1" s="343" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="344"/>
-      <c r="S1" s="344"/>
-      <c r="T1" s="344"/>
-      <c r="U1" s="344"/>
-      <c r="V1" s="340" t="s">
+      <c r="M1" s="360"/>
+      <c r="N1" s="360"/>
+      <c r="O1" s="360"/>
+      <c r="P1" s="360"/>
+      <c r="Q1" s="355" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="356"/>
+      <c r="S1" s="356"/>
+      <c r="T1" s="356"/>
+      <c r="U1" s="356"/>
+      <c r="V1" s="352" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="341"/>
-      <c r="X1" s="341"/>
-      <c r="Y1" s="341"/>
-      <c r="Z1" s="342"/>
+      <c r="W1" s="353"/>
+      <c r="X1" s="353"/>
+      <c r="Y1" s="353"/>
+      <c r="Z1" s="354"/>
     </row>
     <row r="2" spans="1:26" s="80" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -11242,9 +11238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C01FEA-44D9-B84E-A2C5-7D2C4B19A0B7}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11274,50 +11268,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="353" t="s">
+      <c r="B1" s="365" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="354"/>
-      <c r="D1" s="360" t="s">
+      <c r="C1" s="366"/>
+      <c r="D1" s="372" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="361"/>
-      <c r="F1" s="360" t="s">
+      <c r="E1" s="373"/>
+      <c r="F1" s="372" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="361"/>
-      <c r="H1" s="362" t="s">
+      <c r="G1" s="373"/>
+      <c r="H1" s="374" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="363"/>
-      <c r="J1" s="362" t="s">
+      <c r="I1" s="375"/>
+      <c r="J1" s="374" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="363"/>
-      <c r="L1" s="355" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="356"/>
-      <c r="N1" s="355" t="s">
+      <c r="K1" s="375"/>
+      <c r="L1" s="367" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="368"/>
+      <c r="N1" s="367" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="356"/>
-      <c r="P1" s="358" t="s">
+      <c r="O1" s="368"/>
+      <c r="P1" s="370" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="359"/>
-      <c r="R1" s="358" t="s">
+      <c r="Q1" s="371"/>
+      <c r="R1" s="370" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="359"/>
-      <c r="T1" s="357" t="s">
+      <c r="S1" s="371"/>
+      <c r="T1" s="369" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="352"/>
-      <c r="V1" s="351" t="s">
+      <c r="U1" s="364"/>
+      <c r="V1" s="363" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="352"/>
+      <c r="W1" s="364"/>
       <c r="X1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.3">
@@ -12138,7 +12132,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12176,48 +12170,48 @@
   <sheetData>
     <row r="1" spans="1:29" ht="58" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
-      <c r="B1" s="370" t="s">
+      <c r="B1" s="382" t="s">
         <v>903</v>
       </c>
-      <c r="C1" s="371"/>
-      <c r="D1" s="371"/>
-      <c r="E1" s="372"/>
-      <c r="F1" s="373" t="s">
+      <c r="C1" s="383"/>
+      <c r="D1" s="383"/>
+      <c r="E1" s="384"/>
+      <c r="F1" s="385" t="s">
         <v>904</v>
       </c>
-      <c r="G1" s="374"/>
-      <c r="H1" s="374"/>
-      <c r="I1" s="375"/>
-      <c r="J1" s="373" t="s">
+      <c r="G1" s="386"/>
+      <c r="H1" s="386"/>
+      <c r="I1" s="387"/>
+      <c r="J1" s="385" t="s">
         <v>912</v>
       </c>
-      <c r="K1" s="374"/>
-      <c r="L1" s="374"/>
-      <c r="M1" s="375"/>
-      <c r="N1" s="364" t="s">
+      <c r="K1" s="386"/>
+      <c r="L1" s="386"/>
+      <c r="M1" s="387"/>
+      <c r="N1" s="376" t="s">
         <v>905</v>
       </c>
-      <c r="O1" s="365"/>
-      <c r="P1" s="365"/>
-      <c r="Q1" s="366"/>
-      <c r="R1" s="364" t="s">
+      <c r="O1" s="377"/>
+      <c r="P1" s="377"/>
+      <c r="Q1" s="378"/>
+      <c r="R1" s="376" t="s">
         <v>913</v>
       </c>
-      <c r="S1" s="365"/>
-      <c r="T1" s="365"/>
-      <c r="U1" s="366"/>
-      <c r="V1" s="367" t="s">
+      <c r="S1" s="377"/>
+      <c r="T1" s="377"/>
+      <c r="U1" s="378"/>
+      <c r="V1" s="379" t="s">
         <v>906</v>
       </c>
-      <c r="W1" s="368"/>
-      <c r="X1" s="368"/>
-      <c r="Y1" s="369"/>
-      <c r="Z1" s="368" t="s">
+      <c r="W1" s="380"/>
+      <c r="X1" s="380"/>
+      <c r="Y1" s="381"/>
+      <c r="Z1" s="380" t="s">
         <v>914</v>
       </c>
-      <c r="AA1" s="368"/>
-      <c r="AB1" s="368"/>
-      <c r="AC1" s="369"/>
+      <c r="AA1" s="380"/>
+      <c r="AB1" s="380"/>
+      <c r="AC1" s="381"/>
     </row>
     <row r="2" spans="1:29" ht="61" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="225" t="s">

</xml_diff>